<commit_message>
modification in pay and request
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpace-Mobile-07-12-2021\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/Anudeep/Sprint 1/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0360BF0E-3819-4E65-89D1-76EA5610E03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C825C88-50F4-C64E-8E95-09BAFEA0BA52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -21,15 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -103,9 +94,6 @@
 -ppopUpMsg</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>coyni_mobile.tests.LoginTest,
 testLogin,
 -pemail,
@@ -143,17 +131,6 @@
   </si>
   <si>
     <t>SignUp</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.SignUpTest,
-testSignUp,
--pcreateAccount,
--pfirstName,
--plastName,
--pemail,
--pphoneNumber,
--ppassword,
--pconfirmPassword</t>
   </si>
   <si>
     <t>Verify Create Account with Invalid Data</t>
@@ -184,6 +161,29 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.SignUpTest,
+testSignUp,
+-pcreateAccount,
+-pfirstName,
+-plastName,
+-pemail,
+-pphoneNumber,
+-ppassword,
+-pconfirmPassword,
+-pphoneVerificationHeading,
+-pcode,
+-pemailVerificationHeading,
+-psecureYourAccountHeading,
+-pchoosePinHeading,
+-ppin,
+-pconfirmPinHeading,
+-penableFaceIdHeading,
+-pcreateAccountHeading</t>
   </si>
 </sst>
 </file>
@@ -602,23 +602,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -647,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -670,11 +670,11 @@
         <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -691,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>14</v>
@@ -700,9 +700,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>16</v>
@@ -723,12 +723,12 @@
         <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -749,18 +749,18 @@
         <v>14</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>11</v>
@@ -772,47 +772,47 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>11</v>
@@ -824,10 +824,10 @@
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -861,14 +861,14 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -876,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -884,56 +884,56 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added test script in LoginTest for ForgotPassword
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/Mobile_05_01_2022/coyni-automation/Mobile/coyni_mobile/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-mobile\Clone (06-01-2022)[2]\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7077DE4-E637-AB4E-A7A9-9B3814C7782C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78758825-AF97-45D6-AF7E-5779C0111A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -91,14 +91,6 @@
     <t>forgotPassword</t>
   </si>
   <si>
-    <t xml:space="preserve">coyni_mobile.tests.LoginTest,
-testForgotPassword,
--pforgotHeading,
--pemail,
--pemailOtpHeading
-</t>
-  </si>
-  <si>
     <t>Forgot Password with invalid credentials</t>
   </si>
   <si>
@@ -121,17 +113,6 @@
   </si>
   <si>
     <t>Forgot Password with invalid OTP credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coyni_mobile.tests.LoginTest,
-testForgotPasswordInvalidOTPCredentials,
--pforgotHeading,
--pemail,
--pemailOtpHeading,
--perrMessage,
--pcode,
--presendMessage
-</t>
   </si>
   <si>
     <t>Customer Login with valid credentials</t>
@@ -183,14 +164,6 @@
 -pemail,
 -ppassword,
 -ppin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coyni_mobile.tests.LoginTest,
-testForgotPasswordInvalidEmailCredentials,
--pforgotHeading,
--pemail,
--perrMessage
-</t>
   </si>
   <si>
     <t>coyni_mobile.tests.LoginTest,
@@ -297,6 +270,56 @@
 -pretrieveEmailHeading,
 -pfirstName,
 -plastName</t>
+  </si>
+  <si>
+    <t>forgotPassword-OTP</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.LoginTest,
+testForgotPassword,
+-pforgotHeading,
+-pforgotContentHeading,
+-pemail,
+-pcode,
+-pcreateHeading,
+-pnewPassword,
+-pconfirmPassword,
+-pmessage,
+-pemailOtpHeading</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.LoginTest,
+testForgotPasswordInvalidEmailCredentials,
+-pforgotHeading,
+-pforgotContentHeading,
+-pemail,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.LoginTest,
+testForgotPasswordInvalidOTPCredentials,
+-pforgotHeading,
+-pforgotContentHeading,
+-pemail,
+-pemailOtpHeading,
+-perrMessage,
+-pcode,
+-presendMessage</t>
+  </si>
+  <si>
+    <t>Forgot Password with navigation option</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.LoginTest,
+testForgotPasswordWithNavigationOption,
+-pforgotHeading,
+-pforgotContentHeading,
+-pemail,
+-pemailOtpHeading,
+-pcode,
+-pcreateHeading,
+-pnewPassword,
+-pconfirmPassword</t>
   </si>
 </sst>
 </file>
@@ -749,25 +772,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.83203125" customWidth="1"/>
-    <col min="9" max="9" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.77734375" customWidth="1"/>
+    <col min="9" max="9" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -796,15 +819,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>8</v>
@@ -816,22 +839,22 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
@@ -843,22 +866,22 @@
         <v>3</v>
       </c>
       <c r="G3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="101.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -870,22 +893,22 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="77.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -897,14 +920,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -924,16 +947,16 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="96" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>13</v>
@@ -948,19 +971,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>13</v>
@@ -981,46 +1004,46 @@
         <v>17</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14" t="s">
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14">
-        <v>1</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>8</v>
@@ -1032,22 +1055,22 @@
         <v>1</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>8</v>
@@ -1059,22 +1082,22 @@
         <v>1</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" ht="144" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>23</v>
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>8</v>
@@ -1086,22 +1109,22 @@
         <v>1</v>
       </c>
       <c r="G12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:9" ht="160" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>8</v>
@@ -1113,22 +1136,22 @@
         <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>53</v>
+    <row r="14" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>8</v>
@@ -1140,48 +1163,49 @@
         <v>1</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>54</v>
+        <v>21</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="98.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="161.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1190,13 +1214,39 @@
         <v>9</v>
       </c>
       <c r="F16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="98.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>45</v>
+      <c r="F17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1231,14 +1281,14 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="39.5" customWidth="1"/>
+    <col min="7" max="7" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1254,56 +1304,56 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>

</xml_diff>

<commit_message>
modification in customer test
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-mobile\Clone (06-01-2022)[2]\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/Mobile_07_01_2022/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78758825-AF97-45D6-AF7E-5779C0111A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E6863A-FAC6-3B44-911E-9497F2D154B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -177,37 +177,10 @@
 -pexpAccountHeading</t>
   </si>
   <si>
-    <t>testdata.xls,SignUp</t>
-  </si>
-  <si>
     <t>SignUp</t>
   </si>
   <si>
     <t>Verify Create Account with Invalid Data</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.SignUpTest,
-testCreateAccountInvalidData,
--pcreateAccount,
--pfirstName,
--plastName,
--pemail,
--pphoneNumber,
--ppassword,
--pconfirmPassword,
--perrorMessage,
--pelementName</t>
-  </si>
-  <si>
-    <t>Verify field validation in create account</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.SignUpTest,
-testFieldValidationCreateAccount,
--pfirstName,
--plastName,
--pemail,
--pphoneNumber</t>
   </si>
   <si>
     <t>16</t>
@@ -320,6 +293,22 @@
 -pcreateHeading,
 -pnewPassword,
 -pconfirmPassword</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.SignUpTest,
+testCreateAccountInvalidData,
+-pcreateAccount,
+-pfirstName,
+-plastName,
+-pemail,
+-pphoneNumber,
+-ppassword,
+-pconfirmPassword,
+-perrMessage,
+-pelementName</t>
+  </si>
+  <si>
+    <t>testdata.xls,SignupPage</t>
   </si>
 </sst>
 </file>
@@ -454,10 +443,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,25 +761,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" customWidth="1"/>
-    <col min="9" max="9" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
+    <col min="9" max="9" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -819,12 +808,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>27</v>
@@ -846,12 +835,12 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>27</v>
@@ -873,12 +862,12 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="101.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>27</v>
@@ -900,12 +889,12 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="77.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>27</v>
@@ -927,12 +916,12 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
@@ -947,19 +936,19 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -977,16 +966,16 @@
         <v>17</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -1004,16 +993,16 @@
         <v>17</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
@@ -1031,15 +1020,15 @@
         <v>17</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1062,11 +1051,11 @@
       </c>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1075,25 +1064,25 @@
       <c r="D11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14">
-        <v>1</v>
-      </c>
-      <c r="F11" s="14">
-        <v>1</v>
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1102,25 +1091,25 @@
       <c r="D12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
-        <v>1</v>
+      <c r="E12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -1129,25 +1118,25 @@
       <c r="D13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="14">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14">
-        <v>1</v>
+      <c r="E13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>47</v>
+      <c r="H13" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -1156,25 +1145,25 @@
       <c r="D14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
+      <c r="E14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>49</v>
+      <c r="H14" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1183,70 +1172,44 @@
       <c r="D15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="14">
-        <v>1</v>
-      </c>
-      <c r="F15" s="14">
-        <v>1</v>
+      <c r="E15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" ht="161.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" ht="176" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="G16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
       <c r="H16" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="98.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1281,14 +1244,14 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +1259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1304,56 +1267,56 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>

</xml_diff>

<commit_message>
edit address,edit phone number,edit email
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2022\mobile 16_01_2022\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8688284-189A-4BFE-9FE6-01975313435A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358FDF8F-6A5D-4CAE-AEAE-395A9CDBAB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="99">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -488,6 +488,68 @@
 -pcode,
 -pnewEmailHeading,
 -pexpHeading</t>
+  </si>
+  <si>
+    <t>Verify Edit Phone Number</t>
+  </si>
+  <si>
+    <t>Edit Phone Number</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditPhoneNumber,
+-puserDetailsHeading,
+-ppinHeading,
+-ppin,
+-peditPhoneHeading,
+-pphoneNumber,
+-pnewPhoneNumber,
+-pcurrentPhoneHeading,
+-pcode,
+-pnewPhoneHeading,
+-pexpHeading</t>
+  </si>
+  <si>
+    <t>Verify Edit Address</t>
+  </si>
+  <si>
+    <t>Edit Address</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditAddress,
+-puserDetailsHeading,
+-ppinHeading,
+-ppin,
+-peditAddrHeading,
+-paddLine1,
+-paddline2,
+-pcity,
+-pstate,
+-pzipcode,
+-pcountry,
+-pexpAddress</t>
+  </si>
+  <si>
+    <t>Verify Edit Address with Invalid data</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditAddressWithInvalidData,
+-puserDetailsHeading,
+-ppinHeading,
+-ppin,
+-peditAddrHeading,
+-paddLine1,
+-paddline2,
+-pcity,
+-pstate,
+-pzipcode,
+-perrMessage,
+-pelementName</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -955,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1721,7 +1783,7 @@
         <v>88</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>56</v>
@@ -1743,6 +1805,93 @@
       </c>
       <c r="I28" s="10" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Payment Methods
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2022\mobile 16_01_2022\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpace-20-01-2022Mobile\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358FDF8F-6A5D-4CAE-AEAE-395A9CDBAB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957C56-7628-48FC-A9CF-82991D10E6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="107">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -551,12 +551,58 @@
   <si>
     <t>4</t>
   </si>
+  <si>
+    <t>PaymentMethods</t>
+  </si>
+  <si>
+    <t>testdata.xls,PaymentMethods</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testAddDebitCard,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-pcvvOrCVC,
+-paddressLine1,
+-paddreddLine2,
+-pcity,
+-pstate,
+-pzipCode,
+-pamount</t>
+  </si>
+  <si>
+    <t>Verify Add Debit Card</t>
+  </si>
+  <si>
+    <t>Verify Edit Debit Card In Payment Methods</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testEditDebitCard,
+-pcardNumber,
+-pcardExp,
+-pcvvOrCVC,
+-paddressLine1,
+-paddreddLine2,
+-pcity,
+-pstate,
+-pzipCode</t>
+  </si>
+  <si>
+    <t>Verify Delete Debit Card In Payment Methods</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testDeleteDebitCard,
+-pcardNumber</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,13 +616,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -605,41 +644,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -669,39 +687,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1060,114 +1078,114 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="E3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="77.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="3"/>
@@ -1176,7 +1194,7 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1203,7 +1221,7 @@
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1230,7 +1248,7 @@
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1257,7 +1275,7 @@
       <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1281,172 +1299,172 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <v>1</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="14" t="s">
+      <c r="D11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="14" t="s">
+      <c r="D13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" ht="144" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="D14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="14"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="14" t="s">
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="14"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1464,7 +1482,7 @@
       <c r="G16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1472,28 +1490,28 @@
       <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1501,28 +1519,28 @@
       <c r="A18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="14" t="s">
+      <c r="D18" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1530,28 +1548,28 @@
       <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="14" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="19" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1559,7 +1577,7 @@
       <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1568,19 +1586,19 @@
       <c r="D20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1588,28 +1606,28 @@
       <c r="A21" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="14" t="s">
+      <c r="D21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1617,7 +1635,7 @@
       <c r="A22" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1643,7 +1661,7 @@
       <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1669,7 +1687,7 @@
       <c r="A24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1695,7 +1713,7 @@
       <c r="A25" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1713,10 +1731,10 @@
       <c r="G25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1724,7 +1742,7 @@
       <c r="A26" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1742,10 +1760,10 @@
       <c r="G26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="8" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1753,7 +1771,7 @@
       <c r="A27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1771,10 +1789,10 @@
       <c r="G27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1782,13 +1800,13 @@
       <c r="A28" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1800,10 +1818,10 @@
       <c r="G28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1811,13 +1829,13 @@
       <c r="A29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1829,10 +1847,10 @@
       <c r="G29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1840,13 +1858,13 @@
       <c r="A30" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1858,10 +1876,10 @@
       <c r="G30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I30" s="8" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1869,13 +1887,13 @@
       <c r="A31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>12</v>
+      <c r="B31" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1887,11 +1905,98 @@
       <c r="G31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="8" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1920,10 +2025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621ECD84-1FD9-4C9B-A216-6F85DAE3E9BF}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1954,54 +2059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
+    <row r="20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changes in payment methods -Customer profile -user details-Payment Methods
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpace-20-01-2022Mobile\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957C56-7628-48FC-A9CF-82991D10E6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B4133D-0928-4774-97B2-E661B1AE6D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="109">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -596,6 +596,24 @@
     <t>coyni_mobile.tests.CustomerProfileTest,
 testDeleteDebitCard,
 -pcardNumber</t>
+  </si>
+  <si>
+    <t>Verify Add Credit Card With Invalid Data</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.CustomerProfileTest,
+testAddDebitCardWithInvalidData,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-pcvvOrCVC,
+-paddressLine1,
+-paddreddLine2,
+-pcity,
+-pstate,
+-pzipCode,
+-perrMsg,
+-pelementName</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1975,7 +1993,7 @@
         <v>105</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>100</v>
@@ -1997,6 +2015,35 @@
       </c>
       <c r="I34" s="8" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>